<commit_message>
heating technology update logic added (to be tested)
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_HeatingTechnology_Input_Labor.xlsx
+++ b/projects/test_building/input/Scenario_HeatingTechnology_Input_Labor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="4490" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="6960" yWindow="4485" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -579,20 +579,20 @@
   <dimension ref="A1:AS76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.1796875" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -729,7 +729,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -866,7 +866,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>83.1</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>90.1</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>148.80000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>148.80000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>9</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>95.6</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>174.8</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>174.8</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>213.6</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>45.9</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>156.80000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>80.8</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>9</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>82.9</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9</v>
       </c>
@@ -7442,7 +7442,7 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>9</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9</v>
       </c>
@@ -7990,7 +7990,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9</v>
       </c>
@@ -8127,7 +8127,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>61.2</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9</v>
       </c>
@@ -8812,7 +8812,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9</v>
       </c>
@@ -8949,7 +8949,7 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
@@ -9086,7 +9086,7 @@
         <v>86.8</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>86.8</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>108.2</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9</v>
       </c>
@@ -9497,7 +9497,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>61.2</v>
       </c>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9</v>
       </c>
@@ -9908,7 +9908,7 @@
         <v>86.8</v>
       </c>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9</v>
       </c>
@@ -10045,7 +10045,7 @@
         <v>86.8</v>
       </c>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9</v>
       </c>
@@ -10182,7 +10182,7 @@
         <v>108.2</v>
       </c>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9</v>
       </c>
@@ -10319,7 +10319,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9</v>
       </c>
@@ -10456,7 +10456,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9</v>
       </c>
@@ -10593,7 +10593,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9</v>
       </c>
@@ -10867,7 +10867,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9</v>
       </c>

</xml_diff>